<commit_message>
new file:   "test_prompt_record/1K\351\227\256\351\242\230\345\244\215\346\240\270V1.3.xlsx" 	modified:   "test_prompt_record/\344\272\272\347\261\273\345\255\246\344\271\240\350\247\204\350\214\203\346\226\207\346\241\243\347\232\204\350\277\207\347\250\213\347\273\206\345\214\226.docx" 	new file:   "test_prompt_record/\346\210\220\347\206\237\345\272\246\345\216\237\346\226\207.md" 	new file:   "test_prompt_record/\346\210\220\347\206\237\345\272\246\345\216\237\346\226\207\350\241\250\346\240\274.md" 	new file:   "test_prompt_record/\346\210\220\347\206\237\345\272\246\345\216\237\346\226\207\350\241\250\346\240\274.xlsx" 	modified:   "test_prompt_record/\346\240\207\345\207\206\345\255\246\344\271\240\347\232\204\350\277\207\347\250\213.xlsx"
</commit_message>
<xml_diff>
--- a/test_prompt_record/标准学习的过程.xlsx
+++ b/test_prompt_record/标准学习的过程.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17680"/>
+    <workbookView windowHeight="15240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>意图</t>
   </si>
@@ -44,7 +44,7 @@
     <t>这份文档说了什么内容</t>
   </si>
   <si>
-    <t>《GB/T33136-2016 信息技术服务 数据中心服务能力成熟度模型》的国家标准文件。这份文档详细描述了数据中心服务能力成熟度的模型、框架、评价方法和管理要求。以下是文档的主要内容和学习要点：
+    <t>《GB/T33136-2016 信息技术服务 数据中心服务能力成熟度模型》的主要内容和学习要点：
 1. **标准概述**：
    - 目的：确立数据中心对其提供服务能力实施管理的成熟度。
    - 范围：适用于数据中心自身服务能力构建、监视、测量和评价，以及外部评价机构对数据中心服务能力成熟度的测量和评价。
@@ -74,19 +74,114 @@
     <t>确立数据中心服务能力管理成熟度的目的是什么？</t>
   </si>
   <si>
+    <t>确立数据中心服务能力管理成熟度的目的是为了从数据中心相关方实现收益、控制风险和优化资源的基本诉求出发，确立数据中心的目标以及实现这些目标所应具备的服务能力。具体来说，通过评价数据中心的服务能力，可以：
+帮助数据中心对其提供服务的能力实施管理的成熟度进行评估，从而更好地理解自身的服务能力水平。
+从数据中心相关方的需求出发，确立数据中心的目标，并确保这些目标的实现与数据中心的服务能力相匹配。
+通过评价服务能力的特性，将服务能力划分为不同的能力项，并基于证据对每个能力项的成熟度进行评价。
+通过加权计算单个能力项的成熟度，得出整个数据中心服务能力的成熟度，为数据中心的持续改进和提升提供方向和依据。
+使数据中心能够根据评价结果了解自身与既定成熟度级别的差距，设立改进目标和范围，并采取相应的改进措施。
+这样的评价体系有助于数据中心构建、监视、测量和评价自身的服务能力，同时也适用于外部评价机构对数据中心服务能力成熟度进行测量和评价，以及服务需方在选择数据中心时进行评价。</t>
+  </si>
+  <si>
     <t>为什么需要对数据中心服务能力进行成熟度评价？</t>
   </si>
   <si>
+    <t>对数据中心服务能力进行成熟度评估的原因包括但不限于以下几点：
+ 提升服务质量：通过评估，数据中心可以识别服务能力的优势和不足，从而采取措施提高服务质量。
+ 风险管理：评估有助于识别和控制数据中心运营中的风险，确保数据中心的稳定性和安全性。
+ 资源优化：通过了解服务能力的现状，数据中心可以更有效地分配和利用资源，包括人力、财力和物力。
+ 持续改进：成熟度评估提供了一个持续改进的框架，使数据中心能够逐步提升服务能力，向更高级别的成熟度迈进。
+ 目标设定：评估结果可以帮助数据中心明确其发展目标，制定实现这些目标的策略和行动计划。
+ 合规性验证：对于需要遵守特定法律法规和行业标准的数据中心，成熟度评估可以作为验证合规性的一种手段。
+ 增强信任：第三方评价机构的外部评价可以增加服务需方对数据中心服务能力的信任，有助于建立良好的客户关系。
+ 市场竞争力：通过提升服务能力成熟度，数据中心可以增强其在市场中的竞争力，吸引更多的客户和服务需求。
+ 组织学习和知识管理：评估过程促进了组织内部的学习和知识共享，有助于知识的积累和创新。
+报告和透明度：为管理层和利益相关者提供关于数据中心服务能力透明度的报告，有助于做出更明智的决策。
+综上所述，数据中心服务能力成熟度评估是一个全面的工具，有助于数据中心在多个方面实现改进和发展。</t>
+  </si>
+  <si>
     <t>实施成熟度模型对数据中心的长期发展有何重要性？</t>
   </si>
   <si>
+    <t>实施成熟度模型对数据中心的长期发展具有以下重要性：
+1. **明确发展方向**：成熟度模型为数据中心提供了一个清晰的发展方向和目标，帮助数据中心识别和实现长期战略目标。
+2. **持续改进**：通过定期评估和监控服务能力，数据中心能够持续识别改进机会，确保服务能力的不断提升。
+3. **风险控制**：成熟度模型帮助数据中心更好地理解和管理运营风险，从而减少潜在的负面影响。
+4. **资源优化配置**：通过对服务能力的评估，数据中心可以更有效地分配资源，确保资源利用最大化，支持长期增长。
+5. **增强竞争力**：随着服务能力的提升，数据中心能够在市场中提供更高质量的服务，增强其竞争力。
+6. **客户信任**：通过外部评价和认证，数据中心能够建立和维护客户信任，这对于长期客户关系和品牌声誉至关重要。
+7. **合规性保证**：成熟度模型通常包含对合规性的要求，确保数据中心的运营符合法律法规和行业标准。
+8. **组织文化建设**：实施成熟度模型有助于培养一种以质量为中心的组织文化，这种文化能够支持创新和持续学习。
+9. **技术和创新推动**：成熟度模型鼓励数据中心采用新技术和方法，推动创新，以适应不断变化的技术和市场需求。
+10. **决策支持**：成熟度模型提供了关键的性能指标和数据，帮助管理层做出基于数据的决策，提高决策质量。
+11. **市场适应性**：通过评估和改进，数据中心能够更快地适应市场变化，抓住新的商业机会。
+12. **可持续性**：成熟度模型支持数据中心实现可持续发展，通过优化流程和提高效率来降低成本和环境影响。
+总体而言，实施成熟度模型有助于数据中心建立一个坚实的基础，支持其长期稳定发展，并在不断变化的技术和市场环境中保持领先地位。</t>
+  </si>
+  <si>
     <t>能力域、能力子域和能力项的划分对于数据中心服务能力评价有何作用？</t>
   </si>
   <si>
+    <t>能力域、能力子域和能力项的划分对于数据中心服务能力评价具有以下作用：
+1. **细化评价标准**：能力域、能力子域和能力项的划分为数据中心服务能力评价提供了详细的层次结构，使得评价更加具体和细化。
+2. **全面覆盖**：通过不同层次的划分，可以确保评价覆盖数据中心服务的各个方面，包括战略、运营和组织治理等。
+3. **明确责任和角色**：能力项通常对应具体的活动或流程，这有助于明确每个角色和团队的职责，以及他们在服务能力中的作用。
+4. **促进目标对齐**：能力域和子域的设置有助于确保数据中心的各个部分与总体战略目标保持一致。
+5. **识别改进领域**：通过对能力域和能力子域的评估，数据中心可以识别出需要改进或加强的领域。
+6. **支持决策制定**：评价结果可以为数据中心管理层提供决策支持，帮助他们确定资源分配和改进措施的优先级。
+7. **增强透明度**：清晰的能力划分有助于提高数据中心服务能力的透明度，使内外部利益相关者更容易理解数据中心的运营状况。
+8. **促进持续改进**：能力域和能力子域的划分为持续改进提供了框架，数据中心可以针对特定领域制定改进计划。
+9. **便于比较和基准测试**：通过能力域和能力子域的评价，数据中心可以与行业标准或其他数据中心进行比较，进行基准测试。
+10. **支持定制化服务**：能力项的划分使得数据中心能够根据客户的具体需求提供定制化的服务和解决方案。
+11. **风险管理**：不同能力域和子域的评价结果有助于数据中心识别和管理特定领域内的风险。
+12. **促进知识共享**：能力域和能力子域的明确划分有助于数据中心内部的知识共享和最佳实践的传播。
+通过这种分层的划分，数据中心可以更系统地管理和提升其服务能力，确保服务质量和运营效率，同时为持续的改进和发展提供支持。</t>
+  </si>
+  <si>
     <t>评价指标的低、中、高取值标准是如何确定的，它们对数据中心有何指导意义？</t>
   </si>
   <si>
+    <t>评价指标的低、中、高取值标准是根据每个评价要素的具体表现和实现程度来确定的。这些标准通常基于以下几个方面：
+1. **充分性**：指评价要素是否得到了足够的资源、关注或覆盖。例如，管理人充分性低可能意味着管理职责没有明确分配或履行不充分。
+2. **适宜性**：指评价要素是否适合当前的业务需求和环境。例如，技术适宜性高表明所使用的技术平台和工具不仅充分，而且非常适合当前的业务需求。
+3. **有效性**：特别针对过程评价要素，指过程是否有效执行并达到预期目标。
+4. **稳定性和易用性**：对于技术评价要素，指技术平台的稳定性和用户使用的便捷性。
+5. **认知和认可程度**：对于文化评价要素，指相关方对能力项的认知和接受程度。
+6. **管理和执行策略**：对于政策评价要素，指是否有明确的策略以及这些策略是否得到有效执行。
+7. **支持程度**：对于领导和资源评价要素，指管理层的支持程度以及资源的投入是否足够。
+这些取值标准对数据中心具有以下指导意义：
+- **识别差距**：帮助数据中心识别在不同能力要素上的差距，从而知道需要在哪些方面进行改进。
+- **优先级排序**：根据评价结果，数据中心可以确定改进措施的优先级，集中资源解决最紧迫的问题。
+- **目标设定**：为数据中心提供了明确的目标设定依据，使其能够设定可量化和可实现的改进目标。
+- **持续改进**：通过定期的评价，数据中心可以持续监控和改进服务能力，确保与业务发展同步。
+- **决策支持**：评价结果为管理层提供了决策支持，帮助他们理解当前的服务能力状态和未来的发展方向。
+- **合规性和标准符合性**：确保数据中心的服务能力符合行业标准和法规要求。
+- **风险管理**：通过评价，数据中心可以更好地识别和管理与服务能力相关的风险。
+- **沟通和透明度**：评价指标和结果提供了与内外部利益相关者沟通的基础，增加了运营的透明度。
+- **市场竞争力**：通过提升服务能力，数据中心可以增强其在市场中的竞争力。
+通过这些评价指标和相应的取值标准，数据中心能够更系统地管理和提升其服务能力，确保服务质量和运营效率。</t>
+  </si>
+  <si>
     <t>评价要素权重和能力项权重是如何确定的，它们在成熟度评价中扮演什么角色？</t>
+  </si>
+  <si>
+    <t>评价要素权重和能力项权重的确定通常遵循以下步骤和原则：
+1. **战略对齐**：权重应与数据中心的战略目标和关键业务需求保持一致，确保评价模型能够反映数据中心的优先事项。
+2. **专家判断**：通常由经验丰富的管理层、行业专家或评估团队基于对数据中心运营和业务环境的深入理解来确定权重。
+3. **数据分析**：通过分析历史数据和性能指标，识别对服务能力成熟度影响最大的因素，并据此分配权重。
+4. **利益相关者输入**：收集和考虑数据中心内外部利益相关者的意见和需求，以确保权重设置公平且具有代表性。
+5. **风险评估**：考虑每个评价要素和能力项对数据中心运营的风险影响，高风险领域可能会被赋予更高的权重。
+6. **法规和合规性**：符合行业标准和法规要求的评价要素可能会被赋予更高的权重，以确保数据中心的合规性。
+7. **资源和能力**：考虑数据中心在不同领域的资源投入和能力水平，权重可能会偏向于那些需要更多资源或能力提升的领域。
+8. **持续改进**：权重设置应支持数据中心的持续改进目标，鼓励在关键领域进行改进。
+在成熟度评价中，权重扮演的角色包括：
+- **优先级设定**：权重帮助确定哪些评价要素和能力项对数据中心服务能力成熟度的贡献更大，从而为改进和资源分配设定优先级。
+- **综合评估**：通过加权平均，权重使得评价结果能够综合反映所有相关要素和能力项的重要性，提供一个平衡的评价。
+- **决策支持**：权重为数据中心管理层提供了决策支持，帮助他们识别关键领域并制定相应的策略和行动计划。
+- **目标导向**：权重确保评价模型与数据中心的业务目标和战略方向保持一致，支持目标的实现。
+- **风险管理**：权重有助于识别和管理关键风险领域，确保数据中心能够采取适当的风险缓解措施。
+- **持续监控**：权重可以定期进行调整，以反映数据中心业务环境的变化和持续改进的需要。
+权重的确定是一个动态过程，可能需要根据数据中心的业务发展、市场变化和战略调整进行更新。</t>
   </si>
   <si>
     <t>文档的关键概念有哪些</t>
@@ -167,7 +262,16 @@
     <t>议题1）数据中心服务能力成熟度模型的构建</t>
   </si>
   <si>
-    <t>模型级别的问题</t>
+    <t>数据中心服务能力成熟度模型的构建应该从哪些业务目标和需求出发？</t>
+  </si>
+  <si>
+    <t>如何识别和定义数据中心的关键能力域和能力子域？</t>
+  </si>
+  <si>
+    <t>能力项应如何细分，以确保它们能够全面覆盖数据中心的服务能力？</t>
+  </si>
+  <si>
+    <t>应该采用哪些评价要素和指标来衡量每个能力项的成熟度？</t>
   </si>
   <si>
     <t>模型构成的问题</t>
@@ -825,9 +929,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1357,18 +1464,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.73076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="49.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="71.0909090909091" customWidth="1"/>
-    <col min="3" max="3" width="131.636363636364" customWidth="1"/>
-    <col min="4" max="4" width="100.909090909091" customWidth="1"/>
+    <col min="1" max="1" width="49.3653846153846" customWidth="1"/>
+    <col min="2" max="2" width="71.0865384615385" customWidth="1"/>
+    <col min="3" max="3" width="131.634615384615" customWidth="1"/>
+    <col min="4" max="4" width="100.913461538462" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1393,145 +1500,178 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" ht="152" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:2">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="219" spans="2:3">
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="409.5" spans="2:3">
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="409.5" spans="2:3">
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" ht="409.5" spans="2:3">
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" ht="409.5" spans="2:3">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="299" customHeight="1" spans="1:3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" ht="409.5" spans="1:3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" ht="336" spans="1:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" ht="409.5" spans="1:4">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
       <c r="B18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
       <c r="B19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>